<commit_message>
Rolled back the recent changes
</commit_message>
<xml_diff>
--- a/testdata/InputData.xlsx
+++ b/testdata/InputData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>admin</t>
   </si>
@@ -355,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" activeCellId="1" sqref="A1:B5 F14"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,10 +369,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -380,12 +380,12 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -395,49 +395,9 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
       <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R21" t="s">
-        <v>2</v>
-      </c>
-      <c r="S21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R22" t="s">
-        <v>0</v>
-      </c>
-      <c r="S22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R23" t="s">
-        <v>2</v>
-      </c>
-      <c r="S23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="S25" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>